<commit_message>
commiting after making changes
</commit_message>
<xml_diff>
--- a/RantCell_Automation/testdata/Test_Data.xlsx
+++ b/RantCell_Automation/testdata/Test_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RudreshaC\PycharmProjects\RantCell_Automation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RantCell_Automation_GitHub\rantcellautomation\RantCell_Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3966E5A-95EB-408C-A499-4E50F11B877A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8F0505-0082-4BB9-8977-2E886973A78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="0" windowWidth="23490" windowHeight="15480" activeTab="4" xr2:uid="{06A9FDDF-FB50-4CC3-8BB9-A8CCF9D6EAA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{06A9FDDF-FB50-4CC3-8BB9-A8CCF9D6EAA3}"/>
   </bookViews>
   <sheets>
     <sheet name="MODULES" sheetId="1" r:id="rId1"/>
@@ -17497,8 +17497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11C44D7-04DE-4DDA-8378-A5646C36AA32}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17558,7 +17558,7 @@
         <v>497</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -17631,8 +17631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928F057D-58EA-4FFA-AA2F-6211474061A6}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17691,7 +17691,7 @@
         <v>283</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -17852,6 +17852,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FAD45B4BE7354741A84074D46830D6C1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f4f30467dee99edb05b912a5d0b97d09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4a068b9d-11a3-4816-b27c-9d45efe02682" xmlns:ns4="09f01fee-621e-4da6-be98-a5e92b1afc03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8058d872b016908c2cc5877fed5bc0a6" ns3:_="" ns4:_="">
     <xsd:import namespace="4a068b9d-11a3-4816-b27c-9d45efe02682"/>
@@ -18080,15 +18089,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -18098,6 +18098,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{328EDA9D-1ED0-4A08-90C7-6D724647E028}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{528F916E-B78E-4557-B9D9-B9B52872F756}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18112,14 +18120,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{328EDA9D-1ED0-4A08-90C7-6D724647E028}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>